<commit_message>
Uploading the final project in .pdf extension.
</commit_message>
<xml_diff>
--- a/accuracy_error_average.xlsx
+++ b/accuracy_error_average.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\Desktop\unit4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\Desktop\PC\ESCUELA\9. NOVENO SEMESTRE\2. Datos masivos\DATOS MASIVOS (KONDHUGO)\BigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8329974-4537-4CE0-91BC-BA33995FBE9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AB3645-D814-4EF1-816B-B51E163B2801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="ALGORITHMS AVERAGES" sheetId="1" r:id="rId1"/>
+    <sheet name="SUMMARIZING RESULTS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Error</t>
   </si>
@@ -62,6 +63,9 @@
   <si>
     <t>Support Vector Machine</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
 </sst>
 </file>
 
@@ -70,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +86,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -307,11 +326,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -354,42 +388,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,6 +404,48 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,7 +729,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,7 +773,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4">
@@ -748,7 +788,7 @@
       <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="4">
@@ -765,7 +805,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="1">
         <v>0.87425149700598803</v>
       </c>
@@ -778,7 +818,7 @@
       <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="1">
         <v>0.88201019664967195</v>
       </c>
@@ -793,7 +833,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="1">
         <v>0.88100517368810005</v>
       </c>
@@ -806,7 +846,7 @@
       <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="1">
         <v>0.89786921381337204</v>
       </c>
@@ -821,7 +861,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1">
         <v>0.88657573582196703</v>
       </c>
@@ -834,7 +874,7 @@
       <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="1">
         <v>0.87589158345221096</v>
       </c>
@@ -849,7 +889,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="1">
         <v>0.87321830457614402</v>
       </c>
@@ -862,7 +902,7 @@
       <c r="E6" s="3">
         <v>5</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="1">
         <v>0.89458483754512597</v>
       </c>
@@ -877,7 +917,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="1">
         <v>0.86163051608077701</v>
       </c>
@@ -890,7 +930,7 @@
       <c r="E7" s="3">
         <v>6</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="1">
         <v>0.890350877192982</v>
       </c>
@@ -905,7 +945,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="1">
         <v>0.89513108614232195</v>
       </c>
@@ -918,7 +958,7 @@
       <c r="E8" s="3">
         <v>7</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="1">
         <v>0.88182498130142095</v>
       </c>
@@ -933,7 +973,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1">
         <v>0.888408927285817</v>
       </c>
@@ -946,7 +986,7 @@
       <c r="E9" s="3">
         <v>8</v>
       </c>
-      <c r="G9" s="20"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="1">
         <v>0.88846737481031801</v>
       </c>
@@ -961,7 +1001,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="1">
         <v>0.88510007412898395</v>
       </c>
@@ -974,7 +1014,7 @@
       <c r="E10" s="3">
         <v>9</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="1">
         <v>0.88721804511278102</v>
       </c>
@@ -989,7 +1029,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="10">
         <v>0.88531775018261505</v>
       </c>
@@ -1002,7 +1042,7 @@
       <c r="E11" s="12">
         <v>10</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="10">
         <v>0.88387573964497002</v>
       </c>
@@ -1020,7 +1060,7 @@
       <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="23">
         <f>AVERAGE(B2:B11)</f>
         <v>0.88147854063761277</v>
       </c>
@@ -1028,7 +1068,7 @@
         <f>AVERAGE(C2:C11)</f>
         <v>0.1185214593623862</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="20">
         <f>AVERAGE(D2:D11)</f>
         <v>11.4</v>
       </c>
@@ -1036,7 +1076,7 @@
       <c r="G12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="21">
         <f>AVERAGE(H2:H11)</f>
         <v>0.88624587890020923</v>
       </c>
@@ -1044,7 +1084,7 @@
         <f>AVERAGE(I2:I11)</f>
         <v>0.1137541210997897</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="16">
         <f>AVERAGE(J2:J11)</f>
         <v>12.5</v>
       </c>
@@ -1084,7 +1124,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="4">
@@ -1099,7 +1139,7 @@
       <c r="E15" s="6">
         <v>1</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="33" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="4">
@@ -1116,7 +1156,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="1">
         <v>0.88181120491174203</v>
       </c>
@@ -1129,7 +1169,7 @@
       <c r="E16" s="3">
         <v>2</v>
       </c>
-      <c r="G16" s="26"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1144,7 +1184,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="1">
         <v>0.87436456063906998</v>
       </c>
@@ -1157,7 +1197,7 @@
       <c r="E17" s="3">
         <v>3</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1172,7 +1212,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="1">
         <v>0.89236363636363603</v>
       </c>
@@ -1185,7 +1225,7 @@
       <c r="E18" s="3">
         <v>4</v>
       </c>
-      <c r="G18" s="26"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1200,7 +1240,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1">
         <v>0.89049429657794599</v>
       </c>
@@ -1213,7 +1253,7 @@
       <c r="E19" s="3">
         <v>5</v>
       </c>
-      <c r="G19" s="26"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1228,7 +1268,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="1">
         <v>0.89206576125804105</v>
       </c>
@@ -1241,7 +1281,7 @@
       <c r="E20" s="3">
         <v>6</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="34"/>
       <c r="H20" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1256,7 +1296,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="1">
         <v>0.883636363636363</v>
       </c>
@@ -1269,7 +1309,7 @@
       <c r="E21" s="3">
         <v>7</v>
       </c>
-      <c r="G21" s="26"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1284,7 +1324,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="1">
         <v>0.89578872234118401</v>
       </c>
@@ -1297,7 +1337,7 @@
       <c r="E22" s="3">
         <v>8</v>
       </c>
-      <c r="G22" s="26"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1312,7 +1352,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="1">
         <v>0.88373804267844003</v>
       </c>
@@ -1325,7 +1365,7 @@
       <c r="E23" s="3">
         <v>9</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1340,7 +1380,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="24"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="10">
         <v>0.88760585065434905</v>
       </c>
@@ -1353,7 +1393,7 @@
       <c r="E24" s="12">
         <v>10</v>
       </c>
-      <c r="G24" s="27"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="1">
         <v>0.88837567359507297</v>
       </c>
@@ -1371,7 +1411,7 @@
       <c r="A25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="33">
+      <c r="B25" s="22">
         <f>AVERAGE(B15:B24)</f>
         <v>0.88523347603042934</v>
       </c>
@@ -1379,7 +1419,7 @@
         <f>AVERAGE(C15:C24)</f>
         <v>0.11476652396956959</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="17">
         <f>AVERAGE(D15:D24)</f>
         <v>22.8</v>
       </c>
@@ -1387,7 +1427,7 @@
       <c r="G25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="31">
+      <c r="H25" s="19">
         <f>AVERAGE(H15:H24)</f>
         <v>0.88837567359507297</v>
       </c>
@@ -1395,7 +1435,7 @@
         <f>AVERAGE(I15:I24)</f>
         <v>0.11162432640492601</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J25" s="18">
         <f>AVERAGE(J15:J24)</f>
         <v>31.1</v>
       </c>
@@ -1411,4 +1451,90 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111F7A7A-3122-4D78-93EF-01E9B1542BFB}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="37">
+        <v>0.88139999999999996</v>
+      </c>
+      <c r="C2" s="37">
+        <v>0.11849999999999999</v>
+      </c>
+      <c r="D2" s="37">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0.1137</v>
+      </c>
+      <c r="D3" s="37">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="37">
+        <v>0.88519999999999999</v>
+      </c>
+      <c r="C4" s="37">
+        <v>0.1147</v>
+      </c>
+      <c r="D4" s="37">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="37">
+        <v>0.88829999999999998</v>
+      </c>
+      <c r="C5" s="37">
+        <v>0.1116</v>
+      </c>
+      <c r="D5" s="37">
+        <v>31.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>